<commit_message>
6,1 nota de hj
</commit_message>
<xml_diff>
--- a/Provas/Prova Simulado 1.15/CIS.xlsx
+++ b/Provas/Prova Simulado 1.15/CIS.xlsx
@@ -356,13 +356,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -475,22 +475,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -860,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="C54" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -962,23 +965,23 @@
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="18" t="s">
+      <c r="F13" s="20"/>
+      <c r="G13" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -993,17 +996,17 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="19"/>
+      <c r="G14" s="18"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1020,7 +1023,7 @@
       <c r="C16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="21" t="s">
         <v>42</v>
       </c>
       <c r="G16">
@@ -1030,7 +1033,7 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1040,7 +1043,7 @@
       <c r="C18" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="23" t="s">
         <v>39</v>
       </c>
       <c r="G18">
@@ -1050,7 +1053,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="23" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1060,7 +1063,7 @@
       <c r="C20" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="21" t="s">
         <v>41</v>
       </c>
       <c r="G20">
@@ -1070,7 +1073,7 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1080,7 +1083,7 @@
       <c r="C22" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="21" t="s">
         <v>40</v>
       </c>
       <c r="G22">
@@ -1090,7 +1093,7 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1100,7 +1103,7 @@
       <c r="C24" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="21" t="s">
         <v>43</v>
       </c>
       <c r="G24">
@@ -1110,7 +1113,7 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1120,7 +1123,7 @@
       <c r="C26" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="21" t="s">
         <v>44</v>
       </c>
       <c r="G26">
@@ -1130,7 +1133,7 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1140,7 +1143,7 @@
       <c r="C28" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="21" t="s">
         <v>45</v>
       </c>
       <c r="G28">
@@ -1150,7 +1153,7 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="21" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1158,13 +1161,13 @@
       <c r="C30" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="C31" s="14"/>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="21" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1180,23 +1183,23 @@
       <c r="D34" s="16"/>
     </row>
     <row r="35" spans="1:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="21"/>
-      <c r="G35" s="18" t="s">
+      <c r="F35" s="20"/>
+      <c r="G35" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -1211,17 +1214,17 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
@@ -1242,7 +1245,7 @@
       <c r="C38" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="21" t="s">
         <v>30</v>
       </c>
       <c r="E38" s="16"/>
@@ -1257,7 +1260,7 @@
       <c r="A39" s="14"/>
       <c r="B39" s="15"/>
       <c r="C39" s="16"/>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="21" t="s">
         <v>32</v>
       </c>
       <c r="E39" s="16"/>
@@ -1270,7 +1273,7 @@
       <c r="C40" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="21" t="s">
         <v>66</v>
       </c>
       <c r="E40" s="16"/>
@@ -1283,7 +1286,7 @@
       <c r="A41" s="14"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="21" t="s">
         <v>70</v>
       </c>
       <c r="E41" s="16"/>
@@ -1296,7 +1299,7 @@
       <c r="C42" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="22" t="s">
         <v>67</v>
       </c>
       <c r="E42" s="16"/>
@@ -1309,7 +1312,7 @@
       <c r="A43" s="14"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="22" t="s">
         <v>68</v>
       </c>
       <c r="E43" s="16"/>
@@ -1322,7 +1325,7 @@
       <c r="C44" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E44" s="16"/>
@@ -1335,7 +1338,7 @@
       <c r="A45" s="14"/>
       <c r="B45" s="15"/>
       <c r="C45" s="16"/>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="21" t="s">
         <v>33</v>
       </c>
       <c r="E45" s="16"/>
@@ -1348,7 +1351,7 @@
       <c r="C46" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="21" t="s">
         <v>35</v>
       </c>
       <c r="E46" s="16"/>
@@ -1361,7 +1364,7 @@
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
       <c r="C47" s="16"/>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E47" s="16"/>
@@ -1374,7 +1377,7 @@
       <c r="C48" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="17" t="s">
+      <c r="D48" s="21" t="s">
         <v>37</v>
       </c>
       <c r="E48" s="16"/>
@@ -1386,7 +1389,7 @@
     <row r="49" spans="2:7" ht="51" x14ac:dyDescent="0.2">
       <c r="B49" s="16"/>
       <c r="C49" s="16"/>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="21" t="s">
         <v>48</v>
       </c>
       <c r="E49" s="16"/>
@@ -1446,7 +1449,7 @@
       <c r="C54" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="21" t="s">
         <v>47</v>
       </c>
       <c r="E54" s="16"/>
@@ -1458,7 +1461,7 @@
     <row r="55" spans="2:7" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="21" t="s">
         <v>65</v>
       </c>
       <c r="E55" s="16"/>
@@ -1552,7 +1555,7 @@
       <c r="C63" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D63" s="21" t="s">
         <v>69</v>
       </c>
       <c r="E63" s="16"/>
@@ -1602,23 +1605,23 @@
       <c r="F67" s="16"/>
     </row>
     <row r="68" spans="1:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="18" t="s">
+      <c r="A68" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B68" s="18" t="s">
+      <c r="B68" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="18" t="s">
+      <c r="C68" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D68" s="18" t="s">
+      <c r="D68" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E68" s="20" t="s">
+      <c r="E68" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="21"/>
-      <c r="G68" s="18" t="s">
+      <c r="F68" s="20"/>
+      <c r="G68" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H68" s="1" t="s">
@@ -1633,37 +1636,37 @@
       </c>
     </row>
     <row r="69" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A69" s="19"/>
-      <c r="B69" s="19"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
+      <c r="A69" s="18"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
       <c r="E69" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F69" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G69" s="19"/>
+      <c r="G69" s="18"/>
     </row>
     <row r="71" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="72" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="1:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B73" s="18" t="s">
+      <c r="B73" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C73" s="18" t="s">
+      <c r="C73" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D73" s="18" t="s">
+      <c r="D73" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E73" s="20" t="s">
+      <c r="E73" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F73" s="21"/>
+      <c r="F73" s="20"/>
       <c r="G73" s="7" t="s">
         <v>5</v>
       </c>
@@ -1679,10 +1682,10 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A74" s="19"/>
-      <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
+      <c r="A74" s="18"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
       <c r="E74" s="7" t="s">
         <v>6</v>
       </c>
@@ -1694,22 +1697,22 @@
     <row r="76" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="77" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:10" ht="41.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="18" t="s">
+      <c r="A78" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B78" s="18" t="s">
+      <c r="B78" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C78" s="18" t="s">
+      <c r="C78" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D78" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="20" t="s">
+      <c r="E78" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F78" s="21"/>
+      <c r="F78" s="20"/>
       <c r="G78" s="7" t="s">
         <v>5</v>
       </c>
@@ -1725,10 +1728,10 @@
       </c>
     </row>
     <row r="79" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A79" s="19"/>
-      <c r="B79" s="19"/>
-      <c r="C79" s="19"/>
-      <c r="D79" s="19"/>
+      <c r="A79" s="18"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
       <c r="E79" s="7" t="s">
         <v>6</v>
       </c>
@@ -1739,22 +1742,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:F13"/>
     <mergeCell ref="G35:G36"/>
     <mergeCell ref="A68:A69"/>
     <mergeCell ref="B68:B69"/>
@@ -1767,6 +1754,22 @@
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:F68"/>
     <mergeCell ref="G68:G69"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:F78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>